<commit_message>
Update bulk_RNAseq.xlsx and step6 after correcting gene name GHRL1 to GRHL1
</commit_message>
<xml_diff>
--- a/bulk_RNAseq.xlsx
+++ b/bulk_RNAseq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsun/research/GitHub/JAX_bulk_RNAseq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sliu/Documents/Fred_Hutch/github_repos/JAX_bulk_RNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA16954-2525-8F4F-91ED-20F7F863CAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BB6B99-E398-4D49-9AB7-5E13387F6DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="30120" windowHeight="20260" xr2:uid="{9055350D-7DC5-DA46-B56B-6086DC094532}"/>
+    <workbookView xWindow="5100" yWindow="1280" windowWidth="30120" windowHeight="20260" xr2:uid="{9055350D-7DC5-DA46-B56B-6086DC094532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="81">
   <si>
     <t>Release</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Time points</t>
   </si>
   <si>
-    <t>Cortical brain (dorsal forebrain pattering)</t>
-  </si>
-  <si>
     <t>2024/06 ExEm_brain</t>
   </si>
   <si>
@@ -248,9 +245,6 @@
     <t>EPAS1</t>
   </si>
   <si>
-    <t>GHRL1</t>
-  </si>
-  <si>
     <t>5 genes</t>
   </si>
   <si>
@@ -282,6 +276,9 @@
   </si>
   <si>
     <t>EB Time point</t>
+  </si>
+  <si>
+    <t>Cortical brain (dorsal forebrain patterning)</t>
   </si>
 </sst>
 </file>
@@ -881,106 +878,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>138</xdr:row>
-      <xdr:rowOff>60477</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>78194</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3FFD8A-7DA2-C544-6982-F7EC662BD3A1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15038413" y="30661429"/>
-          <a:ext cx="6612064" cy="4896130"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>20159</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>40316</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>348176</xdr:colOff>
-      <xdr:row>138</xdr:row>
-      <xdr:rowOff>60475</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B18E4797-CD02-C813-2BA7-EA4B23E1AAA9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15058572" y="25762856"/>
-          <a:ext cx="6940080" cy="4898571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>508001</xdr:colOff>
       <xdr:row>176</xdr:row>
@@ -1006,7 +903,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1056,7 +953,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1071,56 +968,6 @@
         <a:xfrm>
           <a:off x="6866064" y="39912270"/>
           <a:ext cx="6150428" cy="4515555"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>46364</xdr:colOff>
-      <xdr:row>163</xdr:row>
-      <xdr:rowOff>49450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>230614</xdr:colOff>
-      <xdr:row>183</xdr:row>
-      <xdr:rowOff>31045</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E85B08F1-0916-0CF7-5FFD-3C3F54D4B2DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10178142" y="36851228"/>
-          <a:ext cx="6012139" cy="4497150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1156,7 +1003,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1171,6 +1018,138 @@
         <a:xfrm>
           <a:off x="2640794" y="46586827"/>
           <a:ext cx="5644444" cy="4213597"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>701343</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>56868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>370574</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>20663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1E3EBEA-9D07-2AC5-BA9C-9E906A4D1BA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15031492" y="31219256"/>
+          <a:ext cx="7175500" cy="5422900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>587613</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>18954</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>447344</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>58950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07A5827A-CBF0-D768-4DE3-DE77C0078BA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14083732" y="25722238"/>
+          <a:ext cx="7366000" cy="5499100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>113731</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>37911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>322239</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>131468</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CDDA4EA-CAC1-EA4D-BC55-6227B8996E6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11107761" y="36886866"/>
+          <a:ext cx="6880747" cy="5097736"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1501,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426FC820-AF24-8A4C-B5DC-DAF2203B1CAC}">
   <dimension ref="A1:W209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U192" sqref="U192"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="AB151" sqref="AB151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1536,12 +1515,12 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -1587,7 +1566,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2">
         <v>12</v>
@@ -1703,7 +1682,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>29</v>
@@ -1971,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -1982,7 +1961,7 @@
         <v>28</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -1999,30 +1978,30 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="I52" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -2047,13 +2026,13 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D56" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E56" s="2">
         <v>3</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I56" s="2">
         <v>3</v>
@@ -2064,13 +2043,13 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D57" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E57" s="2">
         <v>3</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I57" s="2">
         <v>0</v>
@@ -2081,7 +2060,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D58" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E58" s="2">
         <v>3</v>
@@ -2089,7 +2068,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D59" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E59" s="2">
         <v>3</v>
@@ -2106,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -2117,7 +2096,7 @@
         <v>48</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -2128,58 +2107,58 @@
         <v>9</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C87" s="2" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="F87" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C88" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="H88" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="I88" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I88" s="2" t="s">
+      <c r="J88" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K88" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="L88" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K88" s="2" t="s">
+      <c r="M88" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L88" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M88" s="2" t="s">
+      <c r="N88" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="N88" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E90" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J90" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J90" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -2195,7 +2174,7 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D92" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E92" s="2">
         <v>0</v>
@@ -2204,7 +2183,7 @@
         <v>3</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J92" s="2">
         <v>3</v>
@@ -2213,7 +2192,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D93" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E93" s="2">
         <v>3</v>
@@ -2222,7 +2201,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J93" s="2">
         <v>3</v>
@@ -2230,7 +2209,7 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I94" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J94" s="2">
         <v>3</v>
@@ -2238,7 +2217,7 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I95" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J95" s="2">
         <v>3</v>
@@ -2246,7 +2225,7 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I96" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J96" s="2">
         <v>3</v>
@@ -2254,7 +2233,7 @@
     </row>
     <row r="97" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I97" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J97" s="2">
         <v>3</v>
@@ -2262,7 +2241,7 @@
     </row>
     <row r="98" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I98" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J98" s="2">
         <v>3</v>
@@ -2270,7 +2249,7 @@
     </row>
     <row r="99" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I99" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J99" s="2">
         <v>3</v>
@@ -2278,7 +2257,7 @@
     </row>
     <row r="100" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I100" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J100" s="2">
         <v>3</v>
@@ -2289,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="B120" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -2303,7 +2282,7 @@
         <v>33</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -2314,12 +2293,12 @@
         <v>9</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C123" s="2" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>33</v>
@@ -2327,7 +2306,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C124" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F124" s="3" t="s">
         <v>17</v>
@@ -2336,7 +2315,7 @@
         <v>12</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="I124" s="2" t="s">
         <v>15</v>
@@ -2352,10 +2331,10 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E127" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I127" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -2374,7 +2353,7 @@
         <v>3</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I129" s="2">
         <v>3</v>
@@ -2385,7 +2364,7 @@
     </row>
     <row r="130" spans="4:10" x14ac:dyDescent="0.2">
       <c r="H130" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I130" s="2">
         <v>3</v>
@@ -2401,7 +2380,7 @@
     </row>
     <row r="132" spans="4:10" x14ac:dyDescent="0.2">
       <c r="H132" s="2" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="I132" s="2">
         <v>3</v>
@@ -2420,10 +2399,10 @@
         <v>0</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.2">
@@ -2434,7 +2413,7 @@
         <v>36</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
@@ -2445,20 +2424,20 @@
         <v>9</v>
       </c>
       <c r="G164" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C165" s="2" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C166" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F166" s="3" t="s">
         <v>17</v>
@@ -2467,7 +2446,7 @@
         <v>12</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="I166" s="2" t="s">
         <v>15</v>
@@ -2480,15 +2459,15 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F168" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E170" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I170" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.2">
@@ -2507,10 +2486,10 @@
         <v>3</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I172" s="2">
         <v>3</v>
@@ -2527,7 +2506,7 @@
         <v>3</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I173" s="2">
         <v>3</v>
@@ -2543,7 +2522,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H175" s="2" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="I175" s="2">
         <v>3</v>
@@ -2562,10 +2541,10 @@
         <v>0</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.2">
@@ -2576,7 +2555,7 @@
         <v>21</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.2">
@@ -2586,20 +2565,20 @@
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C204" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C205" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F207" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K207" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add 2024_10 release NW_RNAseq_1 analysis and some updates for 2024_09 release UCSF_Bulk_EB_Timecourse analysis
</commit_message>
<xml_diff>
--- a/bulk_RNAseq.xlsx
+++ b/bulk_RNAseq.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sliu/Documents/Fred_Hutch/github_repos/JAX_bulk_RNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BB6B99-E398-4D49-9AB7-5E13387F6DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9769267-E62E-A942-AC99-504BF42B550E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="1280" windowWidth="30120" windowHeight="20260" xr2:uid="{9055350D-7DC5-DA46-B56B-6086DC094532}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
   <si>
     <t>Release</t>
   </si>
@@ -279,6 +279,42 @@
   </si>
   <si>
     <t>Cortical brain (dorsal forebrain patterning)</t>
+  </si>
+  <si>
+    <t>2024/10</t>
+  </si>
+  <si>
+    <t>NW_RNAseq_1</t>
+  </si>
+  <si>
+    <t>parental_cell_line_name</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>OCM_108</t>
+  </si>
+  <si>
+    <t>RBBP4</t>
+  </si>
+  <si>
+    <t>OCP74G</t>
+  </si>
+  <si>
+    <t>CHD1</t>
+  </si>
+  <si>
+    <t>treatments</t>
+  </si>
+  <si>
+    <t>DMSO</t>
+  </si>
+  <si>
+    <t>Auxin_6h</t>
+  </si>
+  <si>
+    <t>Auxin_24h</t>
   </si>
 </sst>
 </file>
@@ -1158,6 +1194,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>265373</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>56865</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>113731</xdr:colOff>
+      <xdr:row>253</xdr:row>
+      <xdr:rowOff>54886</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA2B871B-DF9B-F54C-9109-7B8FB68C4FF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5497015" y="52828208"/>
+          <a:ext cx="6444776" cy="4774738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1478,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426FC820-AF24-8A4C-B5DC-DAF2203B1CAC}">
-  <dimension ref="A1:W209"/>
+  <dimension ref="A1:W244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="AB151" sqref="AB151"/>
+    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="Q235" sqref="Q235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2624,6 +2704,72 @@
         <v>3</v>
       </c>
     </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B235" s="2">
+        <v>12</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C237" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C238" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C239" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C241" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C242" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C243" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C244" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
minor update to the knockout strategy for 2024_10 NW_RNAseq_1 in bulk_RNAseq.xlsx
</commit_message>
<xml_diff>
--- a/bulk_RNAseq.xlsx
+++ b/bulk_RNAseq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sliu/Documents/Fred_Hutch/github_repos/JAX_bulk_RNAseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9769267-E62E-A942-AC99-504BF42B550E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B8E5BE-1A9B-DE4A-BFD0-86361174DB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="1280" windowWidth="30120" windowHeight="20260" xr2:uid="{9055350D-7DC5-DA46-B56B-6086DC094532}"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="30120" windowHeight="16620" xr2:uid="{9055350D-7DC5-DA46-B56B-6086DC094532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="94">
   <si>
     <t>Release</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>Auxin_24h</t>
+  </si>
+  <si>
+    <t>AID</t>
   </si>
 </sst>
 </file>
@@ -1560,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426FC820-AF24-8A4C-B5DC-DAF2203B1CAC}">
   <dimension ref="A1:W244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="Q235" sqref="Q235"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="C235" sqref="C235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2723,7 +2726,7 @@
         <v>12</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add June 2025 release JAX RNAseq 08-11
</commit_message>
<xml_diff>
--- a/bulk_RNAseq.xlsx
+++ b/bulk_RNAseq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sliu/Documents/Fred_Hutch/github_repos/JAX_bulk_RNAseq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byu2/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B8E5BE-1A9B-DE4A-BFD0-86361174DB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43702067-BBB7-504C-A181-0600D8ADAEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="500" windowWidth="30120" windowHeight="16620" xr2:uid="{9055350D-7DC5-DA46-B56B-6086DC094532}"/>
+    <workbookView xWindow="1260" yWindow="500" windowWidth="49940" windowHeight="28300" xr2:uid="{9055350D-7DC5-DA46-B56B-6086DC094532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="137">
   <si>
     <t>Release</t>
   </si>
@@ -318,13 +318,142 @@
   </si>
   <si>
     <t>AID</t>
+  </si>
+  <si>
+    <t>2025/06</t>
+  </si>
+  <si>
+    <t>JAX_RNAseq08</t>
+  </si>
+  <si>
+    <t>WT, PTC</t>
+  </si>
+  <si>
+    <t>fibroblast of villous mesenchyme (CL:0002558)</t>
+  </si>
+  <si>
+    <t>primitive syncytium</t>
+  </si>
+  <si>
+    <t>9 genes</t>
+  </si>
+  <si>
+    <t>MAFB</t>
+  </si>
+  <si>
+    <t>ASCL2</t>
+  </si>
+  <si>
+    <t>DLX3</t>
+  </si>
+  <si>
+    <t>ELF5</t>
+  </si>
+  <si>
+    <t>HIF1A</t>
+  </si>
+  <si>
+    <t>MSX2</t>
+  </si>
+  <si>
+    <t>NR2F2</t>
+  </si>
+  <si>
+    <t>TP63</t>
+  </si>
+  <si>
+    <t>VGLL1</t>
+  </si>
+  <si>
+    <t>ELF5*</t>
+  </si>
+  <si>
+    <t>ASCL2*</t>
+  </si>
+  <si>
+    <t>HIF1A*</t>
+  </si>
+  <si>
+    <t>TP63*</t>
+  </si>
+  <si>
+    <t>ExM Time point</t>
+  </si>
+  <si>
+    <t>JAX_RNAseq09</t>
+  </si>
+  <si>
+    <t>8 genes</t>
+  </si>
+  <si>
+    <t>EMX2</t>
+  </si>
+  <si>
+    <t>FOXG1</t>
+  </si>
+  <si>
+    <t>HES5</t>
+  </si>
+  <si>
+    <t>POU3F1</t>
+  </si>
+  <si>
+    <t>POU3F2</t>
+  </si>
+  <si>
+    <t>SOX1</t>
+  </si>
+  <si>
+    <t>SOX21</t>
+  </si>
+  <si>
+    <t>SP8</t>
+  </si>
+  <si>
+    <t>JAX_RNAseq10</t>
+  </si>
+  <si>
+    <t>WT, KO, PTC</t>
+  </si>
+  <si>
+    <t>endoderm</t>
+  </si>
+  <si>
+    <t>mesoderm</t>
+  </si>
+  <si>
+    <t>3 genes</t>
+  </si>
+  <si>
+    <t>EOMES</t>
+  </si>
+  <si>
+    <t>NKX2-1</t>
+  </si>
+  <si>
+    <t>ENDO Time point</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>MESO Time points</t>
+  </si>
+  <si>
+    <t>JAX_RNAseq11</t>
+  </si>
+  <si>
+    <t>Only WT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cortical brain (dorsal forebrain patterning) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -373,6 +502,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -394,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -408,6 +543,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -873,8 +1009,8 @@
       <xdr:rowOff>40319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>826127</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>5273</xdr:colOff>
       <xdr:row>158</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:to>
@@ -1237,6 +1373,494 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1084147</xdr:colOff>
+      <xdr:row>327</xdr:row>
+      <xdr:rowOff>94663</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>248578</xdr:colOff>
+      <xdr:row>345</xdr:row>
+      <xdr:rowOff>77440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE82284-81CB-F0DA-993B-CCDDB0F0B58A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1084147" y="76062346"/>
+          <a:ext cx="5096260" cy="4164484"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>699138</xdr:colOff>
+      <xdr:row>327</xdr:row>
+      <xdr:rowOff>15487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>179125</xdr:colOff>
+      <xdr:row>345</xdr:row>
+      <xdr:rowOff>154877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9F5B43-2966-A1C3-4565-07D0401BC9DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7451821" y="75983170"/>
+          <a:ext cx="5287914" cy="4321097"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>442027</xdr:colOff>
+      <xdr:row>304</xdr:row>
+      <xdr:rowOff>30975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>39339</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>108414</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB030DC-9036-9E53-6BA1-3C584B54538B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10540076" y="70655365"/>
+          <a:ext cx="6164141" cy="4723781"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>334938</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>216830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>813731</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>108413</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68808723-14AD-F745-6F6A-C9C3BFE91DC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16999816" y="70608903"/>
+          <a:ext cx="6224769" cy="4770242"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>681463</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>179593</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>751778</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>154877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E6042AE-2EC0-066F-8EA1-0CD74FF748C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12421219" y="65460691"/>
+          <a:ext cx="6637144" cy="5086259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>72403</xdr:colOff>
+      <xdr:row>238</xdr:row>
+      <xdr:rowOff>30974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>349095</xdr:colOff>
+      <xdr:row>257</xdr:row>
+      <xdr:rowOff>232315</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F21E02B7-21C3-37A3-48E9-31D2D0AAC161}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16737281" y="55322437"/>
+          <a:ext cx="6022668" cy="4615366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>442030</xdr:colOff>
+      <xdr:row>258</xdr:row>
+      <xdr:rowOff>201341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>39339</xdr:colOff>
+      <xdr:row>279</xdr:row>
+      <xdr:rowOff>46463</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E61A0572-B0BE-DD1B-D57C-78F345E62CD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="18748615" y="60139146"/>
+          <a:ext cx="6164139" cy="4723780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>758902</xdr:colOff>
+      <xdr:row>258</xdr:row>
+      <xdr:rowOff>46463</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>705313</xdr:colOff>
+      <xdr:row>279</xdr:row>
+      <xdr:rowOff>159112</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9A1B632-8407-D9C1-01BB-FDC51C223505}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12498658" y="59984268"/>
+          <a:ext cx="6513240" cy="4991307"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1561,10 +2185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426FC820-AF24-8A4C-B5DC-DAF2203B1CAC}">
-  <dimension ref="A1:W244"/>
+  <dimension ref="A1:AF338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C235" sqref="C235"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="AE275" sqref="AE275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2773,6 +3397,714 @@
         <v>92</v>
       </c>
     </row>
+    <row r="257" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A257" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="258" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A258" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B258" s="2">
+        <v>53</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="259" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="C259" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G259" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="260" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="C260" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F260" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="261" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="C261" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F261" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G261" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H261" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I261" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J261" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K261" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L261" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M261" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="262" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="F262" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K262"/>
+    </row>
+    <row r="263" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="F263" s="7"/>
+    </row>
+    <row r="264" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="E264" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I264" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="265" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="E265" s="1">
+        <v>6</v>
+      </c>
+      <c r="I265" s="1">
+        <v>6</v>
+      </c>
+      <c r="X265"/>
+    </row>
+    <row r="266" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="D266" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E266" s="2">
+        <v>3</v>
+      </c>
+      <c r="H266" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I266" s="2">
+        <v>3</v>
+      </c>
+      <c r="J266" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="D267" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E267" s="2">
+        <v>3</v>
+      </c>
+      <c r="H267" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I267" s="2">
+        <v>3</v>
+      </c>
+      <c r="O267"/>
+    </row>
+    <row r="268" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H268" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I268" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF268"/>
+    </row>
+    <row r="269" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H269" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I269" s="2">
+        <v>3</v>
+      </c>
+      <c r="J269" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="270" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H270" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I270" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H271" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I271" s="2">
+        <v>3</v>
+      </c>
+      <c r="J271" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="272" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="H272" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I272" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H273" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I273" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H274" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I274" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H275" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I275" s="2">
+        <v>3</v>
+      </c>
+      <c r="J275" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H276" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I276" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H277" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I277" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H278" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I278" s="2">
+        <v>3</v>
+      </c>
+      <c r="J278" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H279" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I279" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A284" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A285" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B285" s="2">
+        <v>39</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C286" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F286" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G286" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C287" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F287" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G287" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H287" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I287" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J287" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K287" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L287" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M287" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F288" s="3"/>
+      <c r="H288" s="3"/>
+      <c r="I288" s="3"/>
+      <c r="L288" s="3"/>
+    </row>
+    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E289" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E290" s="1">
+        <v>8</v>
+      </c>
+      <c r="F290" s="1">
+        <v>9</v>
+      </c>
+      <c r="G290" s="1">
+        <v>11</v>
+      </c>
+      <c r="H290" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D291" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E291" s="2">
+        <v>0</v>
+      </c>
+      <c r="F291" s="2">
+        <v>0</v>
+      </c>
+      <c r="G291" s="2">
+        <v>0</v>
+      </c>
+      <c r="H291" s="2">
+        <v>3</v>
+      </c>
+      <c r="I291" s="7"/>
+    </row>
+    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D292" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E292" s="2">
+        <v>3</v>
+      </c>
+      <c r="F292" s="2">
+        <v>0</v>
+      </c>
+      <c r="G292" s="2">
+        <v>0</v>
+      </c>
+      <c r="H292" s="2">
+        <v>0</v>
+      </c>
+      <c r="I292" s="1"/>
+    </row>
+    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D293" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E293" s="2">
+        <v>0</v>
+      </c>
+      <c r="F293" s="2">
+        <v>0</v>
+      </c>
+      <c r="G293" s="2">
+        <v>3</v>
+      </c>
+      <c r="H293" s="2">
+        <v>0</v>
+      </c>
+      <c r="P293"/>
+    </row>
+    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D294" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E294" s="2">
+        <v>3</v>
+      </c>
+      <c r="F294" s="2">
+        <v>0</v>
+      </c>
+      <c r="G294" s="2">
+        <v>0</v>
+      </c>
+      <c r="H294" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D295" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E295" s="2">
+        <v>0</v>
+      </c>
+      <c r="F295" s="2">
+        <v>0</v>
+      </c>
+      <c r="G295" s="2">
+        <v>3</v>
+      </c>
+      <c r="H295" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D296" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E296" s="2">
+        <v>0</v>
+      </c>
+      <c r="F296" s="2">
+        <v>0</v>
+      </c>
+      <c r="G296" s="2">
+        <v>3</v>
+      </c>
+      <c r="H296" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D297" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E297" s="2">
+        <v>3</v>
+      </c>
+      <c r="F297" s="2">
+        <v>0</v>
+      </c>
+      <c r="G297" s="2">
+        <v>0</v>
+      </c>
+      <c r="H297" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D298" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E298" s="2">
+        <v>0</v>
+      </c>
+      <c r="F298" s="2">
+        <v>3</v>
+      </c>
+      <c r="G298" s="2">
+        <v>0</v>
+      </c>
+      <c r="H298" s="2">
+        <v>0</v>
+      </c>
+      <c r="J298" s="9"/>
+    </row>
+    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D299" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E299" s="2">
+        <v>6</v>
+      </c>
+      <c r="F299" s="2">
+        <v>3</v>
+      </c>
+      <c r="G299" s="2">
+        <v>3</v>
+      </c>
+      <c r="H299" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J302" s="9"/>
+    </row>
+    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A304" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="305" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A305" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B305" s="2">
+        <v>15</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="306" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C306" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E306" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="307" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C307" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D307" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E307" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="308" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C308" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D308" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F308" s="3"/>
+      <c r="G308" s="3"/>
+      <c r="J308" s="3"/>
+    </row>
+    <row r="310" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="E310" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I310" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="311" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="E311" s="1">
+        <v>5</v>
+      </c>
+      <c r="I311" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="312" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D312" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E312" s="2">
+        <v>3</v>
+      </c>
+      <c r="F312" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H312" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I312" s="2">
+        <v>3</v>
+      </c>
+      <c r="J312" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="313" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D313" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E313" s="2">
+        <v>3</v>
+      </c>
+      <c r="F313" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H313" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I313" s="2">
+        <v>3</v>
+      </c>
+      <c r="U313"/>
+    </row>
+    <row r="314" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D314" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E314" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L316"/>
+    </row>
+    <row r="317" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="J317" s="9"/>
+    </row>
+    <row r="319" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A319" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="320" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A320" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B320" s="2">
+        <v>18</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="321" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C321" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F321" s="1"/>
+      <c r="G321" s="6"/>
+    </row>
+    <row r="322" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C322" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="323" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="F323" s="3"/>
+      <c r="H323" s="3"/>
+      <c r="I323" s="3"/>
+      <c r="L323" s="3"/>
+    </row>
+    <row r="324" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="E324" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I324" s="7"/>
+    </row>
+    <row r="325" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="E325" s="1">
+        <v>3</v>
+      </c>
+      <c r="F325" s="1">
+        <v>4</v>
+      </c>
+      <c r="G325" s="1">
+        <v>5</v>
+      </c>
+      <c r="H325" s="1">
+        <v>20</v>
+      </c>
+      <c r="I325" s="1">
+        <v>25</v>
+      </c>
+      <c r="J325" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="326" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="D326" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E326" s="2">
+        <v>3</v>
+      </c>
+      <c r="F326" s="2">
+        <v>3</v>
+      </c>
+      <c r="G326" s="2">
+        <v>3</v>
+      </c>
+      <c r="H326" s="2">
+        <v>3</v>
+      </c>
+      <c r="I326" s="2">
+        <v>3</v>
+      </c>
+      <c r="J326" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="331" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="J331" s="9"/>
+    </row>
+    <row r="335" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="J335" s="9"/>
+    </row>
+    <row r="336" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="L336"/>
+    </row>
+    <row r="338" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J338" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>